<commit_message>
upload assignment 1 answer, update excel tutorial
</commit_message>
<xml_diff>
--- a/public/files/Excel Tutorial.xlsx
+++ b/public/files/Excel Tutorial.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric Dong\Dropbox\Work\Gooder\PhD\TA\MBAS 821\Shared files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bus-vc\Desktop\Eric\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7560EC8A-6F86-4EFB-A0C1-AB427554B38A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{17E60DD9-5553-4EDE-9FB5-D9FE9DB54D85}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18756" windowHeight="8136" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="NPV and IRR" sheetId="1" r:id="rId1"/>
+    <sheet name="Ass1Q5" sheetId="5" r:id="rId2"/>
+    <sheet name="YTM" sheetId="2" r:id="rId3"/>
+    <sheet name="DCF" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
   <si>
     <t>Year</t>
   </si>
@@ -48,17 +50,139 @@
   </si>
   <si>
     <t>IRR</t>
+  </si>
+  <si>
+    <t>Tax rate</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>Manufacturing Costs</t>
+  </si>
+  <si>
+    <t>Marketing Costs</t>
+  </si>
+  <si>
+    <t>Inventory</t>
+  </si>
+  <si>
+    <t>Account Receivables</t>
+  </si>
+  <si>
+    <t>CAPEX</t>
+  </si>
+  <si>
+    <t>EBIT</t>
+  </si>
+  <si>
+    <t>EBIT x (1-Tc)</t>
+  </si>
+  <si>
+    <t>NWC</t>
+  </si>
+  <si>
+    <t>Change in NWC</t>
+  </si>
+  <si>
+    <t>FCF</t>
+  </si>
+  <si>
+    <t>OCF</t>
+  </si>
+  <si>
+    <t>Depreciation</t>
+  </si>
+  <si>
+    <t>Face value</t>
+  </si>
+  <si>
+    <t>Coupon rate</t>
+  </si>
+  <si>
+    <t>Number of coupon payments per year</t>
+  </si>
+  <si>
+    <t>Maturity (years)</t>
+  </si>
+  <si>
+    <t>CPN</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>effective YTM per period</t>
+  </si>
+  <si>
+    <t>YTM (APR)</t>
+  </si>
+  <si>
+    <t>Effective YTM per period</t>
+  </si>
+  <si>
+    <t>YTM(APR)</t>
+  </si>
+  <si>
+    <t>Price of bond</t>
+  </si>
+  <si>
+    <t>(in $ million)</t>
+  </si>
+  <si>
+    <t>growth rate</t>
+  </si>
+  <si>
+    <t>EBIT (9% sales)</t>
+  </si>
+  <si>
+    <t>Tax</t>
+  </si>
+  <si>
+    <t>change in NWC</t>
+  </si>
+  <si>
+    <t>CAPEX - Dep</t>
+  </si>
+  <si>
+    <t>Terminal Value (at 2011)</t>
+  </si>
+  <si>
+    <t>Enterprise Value</t>
+  </si>
+  <si>
+    <t>Cash</t>
+  </si>
+  <si>
+    <t>Debt</t>
+  </si>
+  <si>
+    <t>Shares Outstanding</t>
+  </si>
+  <si>
+    <t>Share Price</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="4">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;* #,##0_-;[Red]&quot;$&quot;* \(#,##0\)_-"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -86,7 +210,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -94,6 +218,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="6" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="8" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -545,20 +677,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7E691EA-3531-44DB-ABA6-57223410B47E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13:T19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="3"/>
-    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="3"/>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -626,7 +758,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -713,7 +845,7 @@
         <v>126347.50976878197</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -721,7 +853,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
@@ -730,7 +862,7 @@
         <v>-394395.79712080187</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -739,7 +871,7 @@
         <v>4.5167513239157353E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="P15" s="2"/>
     </row>
   </sheetData>
@@ -747,4 +879,834 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D4">
+        <v>2021</v>
+      </c>
+      <c r="E4">
+        <v>2022</v>
+      </c>
+      <c r="F4">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="6">
+        <v>10000</v>
+      </c>
+      <c r="E5" s="6">
+        <v>12000</v>
+      </c>
+      <c r="F5" s="6">
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="6">
+        <v>3000</v>
+      </c>
+      <c r="E6" s="6">
+        <v>4000</v>
+      </c>
+      <c r="F6" s="6">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="6">
+        <v>2000</v>
+      </c>
+      <c r="E7" s="6">
+        <v>0</v>
+      </c>
+      <c r="F7" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C8" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="7">
+        <f>$B$3/3</f>
+        <v>2000</v>
+      </c>
+      <c r="E8" s="7">
+        <f t="shared" ref="E8:F8" si="0">$B$3/3</f>
+        <v>2000</v>
+      </c>
+      <c r="F8" s="7">
+        <f t="shared" si="0"/>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="6">
+        <v>1200</v>
+      </c>
+      <c r="E9" s="6">
+        <v>1400</v>
+      </c>
+      <c r="F9" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="6">
+        <v>1000</v>
+      </c>
+      <c r="E10" s="6">
+        <v>1200</v>
+      </c>
+      <c r="F10" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="6">
+        <f>D5-D6-D7-D8</f>
+        <v>3000</v>
+      </c>
+      <c r="E12" s="6">
+        <f t="shared" ref="E12:F12" si="1">E5-E6-E7-E8</f>
+        <v>6000</v>
+      </c>
+      <c r="F12" s="6">
+        <f t="shared" si="1"/>
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C13" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="9">
+        <f>D12*(1-$B$1)</f>
+        <v>1800</v>
+      </c>
+      <c r="E13" s="9">
+        <f t="shared" ref="E13:F13" si="2">E12*(1-$B$1)</f>
+        <v>3600</v>
+      </c>
+      <c r="F13" s="9">
+        <f t="shared" si="2"/>
+        <v>4200</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C15" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="7">
+        <f xml:space="preserve"> D13+D8</f>
+        <v>3800</v>
+      </c>
+      <c r="E15" s="7">
+        <f t="shared" ref="E15:F15" si="3" xml:space="preserve"> E13+E8</f>
+        <v>5600</v>
+      </c>
+      <c r="F15" s="7">
+        <f t="shared" si="3"/>
+        <v>6200</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C17" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="6">
+        <f>D9+D10</f>
+        <v>2200</v>
+      </c>
+      <c r="E17" s="6">
+        <f t="shared" ref="E17:F17" si="4">E9+E10</f>
+        <v>2600</v>
+      </c>
+      <c r="F17" s="6">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C18" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="7">
+        <f>D17</f>
+        <v>2200</v>
+      </c>
+      <c r="E18" s="7">
+        <f>E17-D17</f>
+        <v>400</v>
+      </c>
+      <c r="F18" s="7">
+        <f>F17-E17</f>
+        <v>-2600</v>
+      </c>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="6">
+        <f>D15-D18</f>
+        <v>1600</v>
+      </c>
+      <c r="E20" s="6">
+        <f t="shared" ref="E20:F20" si="5">E15-E18</f>
+        <v>5200</v>
+      </c>
+      <c r="F20" s="6">
+        <f t="shared" si="5"/>
+        <v>8800</v>
+      </c>
+    </row>
+    <row r="22" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C22" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="8">
+        <f>NPV(B2,D20:F20)-B3</f>
+        <v>7220.6298064639341</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L32"/>
+  <sheetViews>
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="32.33203125" customWidth="1"/>
+    <col min="8" max="8" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2">
+        <f>B1*B2/B3</f>
+        <v>25</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="5"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3">
+        <f>B4*B3</f>
+        <v>10</v>
+      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="5"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="5"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5">
+        <v>900</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="5"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="4">
+        <f>RATE(F3,F2,-B5,B1)</f>
+        <v>3.7155107773155442E-2</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="5"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="4">
+        <f>B6*2</f>
+        <v>7.4310215546310884E-2</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="5"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="5"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9">
+        <v>4</v>
+      </c>
+      <c r="G9">
+        <v>5</v>
+      </c>
+      <c r="H9">
+        <v>6</v>
+      </c>
+      <c r="I9">
+        <v>7</v>
+      </c>
+      <c r="J9">
+        <v>8</v>
+      </c>
+      <c r="K9">
+        <v>9</v>
+      </c>
+      <c r="L9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>-900</v>
+      </c>
+      <c r="C10">
+        <v>25</v>
+      </c>
+      <c r="D10">
+        <v>25</v>
+      </c>
+      <c r="E10">
+        <v>25</v>
+      </c>
+      <c r="F10">
+        <v>25</v>
+      </c>
+      <c r="G10">
+        <v>25</v>
+      </c>
+      <c r="H10">
+        <v>25</v>
+      </c>
+      <c r="I10">
+        <v>25</v>
+      </c>
+      <c r="J10">
+        <v>25</v>
+      </c>
+      <c r="K10">
+        <v>25</v>
+      </c>
+      <c r="L10">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="4">
+        <f>IRR(B10:L10)</f>
+        <v>3.7155107773378937E-2</v>
+      </c>
+      <c r="F11" s="4"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="5"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="4">
+        <f>B11*B3</f>
+        <v>7.4310215546757874E-2</v>
+      </c>
+      <c r="H12" s="2"/>
+      <c r="I12" s="5"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H13" s="2"/>
+      <c r="I13" s="5"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H14" s="2"/>
+      <c r="I14" s="5"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H15" s="2"/>
+      <c r="I15" s="5"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H16" s="2"/>
+      <c r="I16" s="5"/>
+    </row>
+    <row r="17" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H17" s="2"/>
+      <c r="I17" s="5"/>
+    </row>
+    <row r="18" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H18" s="2"/>
+      <c r="I18" s="5"/>
+    </row>
+    <row r="19" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H19" s="2"/>
+      <c r="I19" s="5"/>
+    </row>
+    <row r="20" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H20" s="2"/>
+      <c r="I20" s="5"/>
+    </row>
+    <row r="21" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H21" s="2"/>
+      <c r="I21" s="5"/>
+    </row>
+    <row r="22" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H22" s="2"/>
+      <c r="I22" s="5"/>
+    </row>
+    <row r="23" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H23" s="2"/>
+    </row>
+    <row r="24" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H27" s="2"/>
+    </row>
+    <row r="28" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H28" s="2"/>
+    </row>
+    <row r="29" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H29" s="2"/>
+    </row>
+    <row r="30" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H30" s="2"/>
+    </row>
+    <row r="31" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H31" s="2"/>
+    </row>
+    <row r="32" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H32" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1">
+        <v>2005</v>
+      </c>
+      <c r="C1">
+        <v>2006</v>
+      </c>
+      <c r="D1">
+        <v>2007</v>
+      </c>
+      <c r="E1">
+        <v>2008</v>
+      </c>
+      <c r="F1">
+        <v>2009</v>
+      </c>
+      <c r="G1">
+        <v>2010</v>
+      </c>
+      <c r="H1">
+        <v>2011</v>
+      </c>
+      <c r="K1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" s="2">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="5">
+        <v>518</v>
+      </c>
+      <c r="C2" s="5">
+        <f>B2*(1+C3)</f>
+        <v>564.62</v>
+      </c>
+      <c r="D2" s="5">
+        <f t="shared" ref="D2:H2" si="0">C2*(1+D3)</f>
+        <v>609.78960000000006</v>
+      </c>
+      <c r="E2" s="5">
+        <f t="shared" si="0"/>
+        <v>652.47487200000012</v>
+      </c>
+      <c r="F2" s="5">
+        <f t="shared" si="0"/>
+        <v>691.62336432000018</v>
+      </c>
+      <c r="G2" s="5">
+        <f t="shared" si="0"/>
+        <v>726.20453253600022</v>
+      </c>
+      <c r="H2" s="5">
+        <f t="shared" si="0"/>
+        <v>755.2527138374403</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="E3" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5">
+        <f>C2*9%</f>
+        <v>50.815799999999996</v>
+      </c>
+      <c r="D4" s="5">
+        <f t="shared" ref="D4:H4" si="1">D2*9%</f>
+        <v>54.881064000000002</v>
+      </c>
+      <c r="E4" s="5">
+        <f t="shared" si="1"/>
+        <v>58.722738480000011</v>
+      </c>
+      <c r="F4" s="5">
+        <f t="shared" si="1"/>
+        <v>62.246102788800016</v>
+      </c>
+      <c r="G4" s="5">
+        <f t="shared" si="1"/>
+        <v>65.358407928240013</v>
+      </c>
+      <c r="H4" s="5">
+        <f t="shared" si="1"/>
+        <v>67.972744245369626</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5">
+        <f>C4*(1-$L$1)</f>
+        <v>32.013953999999998</v>
+      </c>
+      <c r="D5" s="5">
+        <f t="shared" ref="D5:H5" si="2">D4*(1-$L$1)</f>
+        <v>34.575070320000002</v>
+      </c>
+      <c r="E5" s="5">
+        <f t="shared" si="2"/>
+        <v>36.995325242400007</v>
+      </c>
+      <c r="F5" s="5">
+        <f t="shared" si="2"/>
+        <v>39.21504475694401</v>
+      </c>
+      <c r="G5" s="5">
+        <f t="shared" si="2"/>
+        <v>41.175796994791206</v>
+      </c>
+      <c r="H5" s="5">
+        <f t="shared" si="2"/>
+        <v>42.822828874582868</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5">
+        <f>(C2-B2)*0.1</f>
+        <v>4.6620000000000008</v>
+      </c>
+      <c r="D6" s="5">
+        <f t="shared" ref="D6:H6" si="3">(D2-C2)*0.1</f>
+        <v>4.5169600000000063</v>
+      </c>
+      <c r="E6" s="5">
+        <f t="shared" si="3"/>
+        <v>4.2685272000000056</v>
+      </c>
+      <c r="F6" s="5">
+        <f t="shared" si="3"/>
+        <v>3.9148492320000061</v>
+      </c>
+      <c r="G6" s="5">
+        <f t="shared" si="3"/>
+        <v>3.458116821600004</v>
+      </c>
+      <c r="H6" s="5">
+        <f t="shared" si="3"/>
+        <v>2.9048181301440081</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5">
+        <f>(C2-B2)*8%</f>
+        <v>3.7296000000000005</v>
+      </c>
+      <c r="D7" s="5">
+        <f t="shared" ref="D7:H7" si="4">(D2-C2)*8%</f>
+        <v>3.6135680000000048</v>
+      </c>
+      <c r="E7" s="5">
+        <f t="shared" si="4"/>
+        <v>3.4148217600000046</v>
+      </c>
+      <c r="F7" s="5">
+        <f t="shared" si="4"/>
+        <v>3.1318793856000049</v>
+      </c>
+      <c r="G7" s="5">
+        <f t="shared" si="4"/>
+        <v>2.7664934572800028</v>
+      </c>
+      <c r="H7" s="5">
+        <f t="shared" si="4"/>
+        <v>2.3238545041152068</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11">
+        <f>C5-C6-C7</f>
+        <v>23.622353999999998</v>
+      </c>
+      <c r="D8" s="11">
+        <f t="shared" ref="D8:H8" si="5">D5-D6-D7</f>
+        <v>26.444542319999993</v>
+      </c>
+      <c r="E8" s="11">
+        <f t="shared" si="5"/>
+        <v>29.311976282399993</v>
+      </c>
+      <c r="F8" s="11">
+        <f t="shared" si="5"/>
+        <v>32.168316139344</v>
+      </c>
+      <c r="G8" s="11">
+        <f t="shared" si="5"/>
+        <v>34.951186715911206</v>
+      </c>
+      <c r="H8" s="11">
+        <f t="shared" si="5"/>
+        <v>37.594156240323656</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="9">
+        <f>H8*(1+0.04)/(0.11 - 0.04)</f>
+        <v>558.54174985623706</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="12">
+        <f>NPV(11%, C8:G8,H8+B10)</f>
+        <v>424.82774186924161</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="9">
+        <f>(B12+B13-B14)/B15</f>
+        <v>24.848940089011506</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
assignment 2 deadline extended
</commit_message>
<xml_diff>
--- a/public/files/Excel Tutorial.xlsx
+++ b/public/files/Excel Tutorial.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bus-vc\Desktop\Eric\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric Dong\Dropbox\Work\Gooder\PhD\Website\web1\static\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0B13E62-1DE1-4994-AD34-B98003E4D01A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18756" windowHeight="8136" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NPV and IRR" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,7 @@
     <sheet name="YTM" sheetId="2" r:id="rId3"/>
     <sheet name="DCF" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -166,7 +167,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
@@ -677,20 +678,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="3"/>
-    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -758,7 +759,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -845,7 +846,7 @@
         <v>126347.50976878197</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -853,7 +854,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
@@ -862,7 +863,7 @@
         <v>-394395.79712080187</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -871,7 +872,7 @@
         <v>4.5167513239157353E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="P15" s="2"/>
     </row>
   </sheetData>
@@ -882,19 +883,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -902,7 +903,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -910,7 +911,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -918,7 +919,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D4">
         <v>2021</v>
       </c>
@@ -929,7 +930,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>6</v>
       </c>
@@ -943,7 +944,7 @@
         <v>14000</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>7</v>
       </c>
@@ -957,7 +958,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>8</v>
       </c>
@@ -971,7 +972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C8" s="9" t="s">
         <v>18</v>
       </c>
@@ -988,7 +989,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>9</v>
       </c>
@@ -1002,7 +1003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>10</v>
       </c>
@@ -1016,7 +1017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>12</v>
       </c>
@@ -1033,7 +1034,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C13" s="9" t="s">
         <v>13</v>
       </c>
@@ -1050,7 +1051,7 @@
         <v>4200</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C15" s="9" t="s">
         <v>17</v>
       </c>
@@ -1067,7 +1068,7 @@
         <v>6200</v>
       </c>
     </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C17" s="10" t="s">
         <v>14</v>
       </c>
@@ -1084,7 +1085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C18" s="9" t="s">
         <v>15</v>
       </c>
@@ -1101,7 +1102,7 @@
         <v>-2600</v>
       </c>
     </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>16</v>
       </c>
@@ -1118,7 +1119,7 @@
         <v>8800</v>
       </c>
     </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>2</v>
       </c>
@@ -1133,21 +1134,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.33203125" customWidth="1"/>
-    <col min="8" max="8" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.28515625" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -1155,7 +1156,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -1172,7 +1173,7 @@
       <c r="H2" s="2"/>
       <c r="I2" s="5"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1189,7 +1190,7 @@
       <c r="H3" s="2"/>
       <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -1199,7 +1200,7 @@
       <c r="H4" s="2"/>
       <c r="I4" s="5"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -1209,7 +1210,7 @@
       <c r="H5" s="2"/>
       <c r="I5" s="5"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -1220,23 +1221,23 @@
       <c r="H6" s="2"/>
       <c r="I6" s="5"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>26</v>
       </c>
       <c r="B7" s="4">
-        <f>B6*2</f>
+        <f>B6*B3</f>
         <v>7.4310215546310884E-2</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="5"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="5"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>0</v>
       </c>
@@ -1271,42 +1272,53 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B10">
+        <f>-B5</f>
         <v>-900</v>
       </c>
       <c r="C10">
+        <f>$F$2</f>
         <v>25</v>
       </c>
       <c r="D10">
+        <f t="shared" ref="D10:K10" si="0">$F$2</f>
         <v>25</v>
       </c>
       <c r="E10">
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="F10">
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="G10">
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="H10">
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="I10">
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="J10">
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="K10">
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="L10">
+        <f>B1+F2</f>
         <v>1025</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1318,7 +1330,7 @@
       <c r="H11" s="2"/>
       <c r="I11" s="5"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -1329,74 +1341,74 @@
       <c r="H12" s="2"/>
       <c r="I12" s="5"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H13" s="2"/>
       <c r="I13" s="5"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H14" s="2"/>
       <c r="I14" s="5"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H15" s="2"/>
       <c r="I15" s="5"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H16" s="2"/>
       <c r="I16" s="5"/>
     </row>
-    <row r="17" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H17" s="2"/>
       <c r="I17" s="5"/>
     </row>
-    <row r="18" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H18" s="2"/>
       <c r="I18" s="5"/>
     </row>
-    <row r="19" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H19" s="2"/>
       <c r="I19" s="5"/>
     </row>
-    <row r="20" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H20" s="2"/>
       <c r="I20" s="5"/>
     </row>
-    <row r="21" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H21" s="2"/>
       <c r="I21" s="5"/>
     </row>
-    <row r="22" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H22" s="2"/>
       <c r="I22" s="5"/>
     </row>
-    <row r="23" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H32" s="2"/>
     </row>
   </sheetData>
@@ -1406,19 +1418,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.33203125" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -1450,7 +1462,7 @@
         <v>0.37</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1482,7 +1494,7 @@
         <v>755.2527138374403</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -1505,7 +1517,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -1535,7 +1547,7 @@
         <v>67.972744245369626</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1565,7 +1577,7 @@
         <v>42.822828874582868</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -1595,7 +1607,7 @@
         <v>2.9048181301440081</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -1625,7 +1637,7 @@
         <v>2.3238545041152068</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>16</v>
       </c>
@@ -1655,7 +1667,7 @@
         <v>37.594156240323656</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -1664,7 +1676,7 @@
         <v>558.54174985623706</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -1673,7 +1685,7 @@
         <v>424.82774186924161</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -1681,7 +1693,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -1689,7 +1701,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>40</v>
       </c>
@@ -1697,7 +1709,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>41</v>
       </c>

</xml_diff>